<commit_message>
designing done , some minor changes and detailing
</commit_message>
<xml_diff>
--- a/public/graph_xl_files/Mohgaon_Univariate_Stationary_1.xlsx
+++ b/public/graph_xl_files/Mohgaon_Univariate_Stationary_1.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithi\OneDrive\Documents\Desktop\data_points\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nithi\OneDrive\Documents\Desktop\data_points\data_points\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4AE5D51E-8B7B-40C9-9BCD-45B9A019254E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2385F21D-DEA4-4052-A1BD-807EC98CEF71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{69A8222A-DC84-4703-8D00-0884BD02670A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B1B32C42-6E2E-47F0-AE77-D15C835DF6F3}"/>
   </bookViews>
   <sheets>
-    <sheet name="1_Mohgaon_NS_RP_RL_data_univari" sheetId="1" r:id="rId1"/>
+    <sheet name="1_Mohgaon_S_RP_RL_data_univaria" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -894,11 +894,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22A9E28C-C860-4CDC-AD33-1FABE6E06D58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0CE9F90-78EF-487A-A36C-5FF274DC418E}">
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,1685 +922,1685 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1810.8145595671699</v>
+        <v>2357.6962121279598</v>
       </c>
       <c r="B2">
-        <v>1458.1685964680501</v>
+        <v>1792.76996480348</v>
       </c>
       <c r="C2">
-        <v>2166.6019176244999</v>
+        <v>2934.43789662779</v>
       </c>
       <c r="D2">
-        <v>1347.98725163738</v>
+        <v>1617.5642688486</v>
       </c>
       <c r="E2">
-        <v>2279.0682022757701</v>
+        <v>3118.24203173572</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2594.4686028117899</v>
+        <v>3196.1695425937701</v>
       </c>
       <c r="B3">
-        <v>2084.2966332622</v>
+        <v>2315.8884029414999</v>
       </c>
       <c r="C3">
-        <v>3128.5794805839701</v>
+        <v>4165.4051748204902</v>
       </c>
       <c r="D3">
-        <v>1928.55980108463</v>
+        <v>2055.3061353142398</v>
       </c>
       <c r="E3">
-        <v>3301.7500806253402</v>
+        <v>4490.9627733667103</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3159.1069997912</v>
+        <v>3804.5658589551299</v>
       </c>
       <c r="B4">
-        <v>2513.2296000249198</v>
+        <v>2663.8221382521401</v>
       </c>
       <c r="C4">
-        <v>3857.4473126702801</v>
+        <v>5139.2761438796497</v>
       </c>
       <c r="D4">
-        <v>2320.0114739566802</v>
+        <v>2338.56690583206</v>
       </c>
       <c r="E4">
-        <v>4088.9217190255999</v>
+        <v>5606.76814133065</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3612.1948107275098</v>
+        <v>4295.1131265444601</v>
       </c>
       <c r="B5">
-        <v>2845.78175707327</v>
+        <v>2928.2062798737902</v>
       </c>
       <c r="C5">
-        <v>4462.7556589366995</v>
+        <v>5972.3332521664197</v>
       </c>
       <c r="D5">
-        <v>2620.2373935252799</v>
+        <v>2549.8265668353902</v>
       </c>
       <c r="E5">
-        <v>4749.7352496357198</v>
+        <v>6579.1010835063998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3995.45817872525</v>
+        <v>4711.58796421016</v>
       </c>
       <c r="B6">
-        <v>3119.7807802504699</v>
+        <v>3142.7182742759801</v>
       </c>
       <c r="C6">
-        <v>4988.4167370894002</v>
+        <v>6712.3480138505802</v>
       </c>
       <c r="D6">
-        <v>2865.5641126681999</v>
+        <v>2718.8076697487299</v>
       </c>
       <c r="E6">
-        <v>5328.3537697955599</v>
+        <v>7455.19463625148</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>4330.1721360042602</v>
+        <v>5076.3908391831901</v>
       </c>
       <c r="B7">
-        <v>3354.0166589311698</v>
+        <v>3323.8281653497702</v>
       </c>
       <c r="C7">
-        <v>5457.3902603650904</v>
+        <v>7384.8144455297597</v>
       </c>
       <c r="D7">
-        <v>3073.8857999965699</v>
+        <v>2859.8352475247002</v>
       </c>
       <c r="E7">
-        <v>5848.04472314744</v>
+        <v>8260.55859988472</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>4628.8511491218096</v>
+        <v>5402.73684310521</v>
       </c>
       <c r="B8">
-        <v>3559.30988523421</v>
+        <v>3480.90210338527</v>
       </c>
       <c r="C8">
-        <v>5883.4644659702899</v>
+        <v>8005.30889886356</v>
       </c>
       <c r="D8">
-        <v>3255.4377643172702</v>
+        <v>2980.9605668424701</v>
       </c>
       <c r="E8">
-        <v>6322.87035516369</v>
+        <v>9010.9410715664908</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>4899.5547792944899</v>
+        <v>5699.1578631812899</v>
       </c>
       <c r="B9">
-        <v>3742.50538367835</v>
+        <v>3619.80283937694</v>
       </c>
       <c r="C9">
-        <v>6275.6769875644404</v>
+        <v>8584.1933636623107</v>
       </c>
       <c r="D9">
-        <v>3416.6581267940901</v>
+        <v>3087.1739900514099</v>
       </c>
       <c r="E9">
-        <v>6762.0982270930399</v>
+        <v>9716.9131617450694</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5147.8126366986598</v>
+        <v>5971.5201541107999</v>
       </c>
       <c r="B10">
-        <v>3908.22722208715</v>
+        <v>3744.4550483497101</v>
       </c>
       <c r="C10">
-        <v>6640.3240745150897</v>
+        <v>9128.7808418940695</v>
       </c>
       <c r="D10">
-        <v>3561.8748967278998</v>
+        <v>3181.7879915631702</v>
       </c>
       <c r="E10">
-        <v>7172.2155192963601</v>
+        <v>10385.995005999401</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>5377.6009144546597</v>
+        <v>6224.0499836282297</v>
       </c>
       <c r="B11">
-        <v>4059.7553583222498</v>
+        <v>3857.6203847967699</v>
       </c>
       <c r="C11">
-        <v>6981.99482147052</v>
+        <v>9644.4631366506692</v>
       </c>
       <c r="D11">
-        <v>3694.1448300219399</v>
+        <v>3267.1161350267798</v>
       </c>
       <c r="E11">
-        <v>7557.9704386071298</v>
+        <v>11023.770595337801</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>5591.88455386647</v>
+        <v>6459.9041166507004</v>
       </c>
       <c r="B12">
-        <v>4199.5059012281799</v>
+        <v>3961.3186622092799</v>
       </c>
       <c r="C12">
-        <v>7304.1528920457904</v>
+        <v>10135.352017072701</v>
       </c>
       <c r="D12">
-        <v>3815.7109688757901</v>
+        <v>3344.8392925176299</v>
       </c>
       <c r="E12">
-        <v>7922.9603072570699</v>
+        <v>11634.5255837023</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>5792.93947008749</v>
+        <v>6681.5094356052005</v>
       </c>
       <c r="B13">
-        <v>4329.31312262954</v>
+        <v>4057.0734135903599</v>
       </c>
       <c r="C13">
-        <v>7609.4863448224396</v>
+        <v>10604.6685704667</v>
       </c>
       <c r="D13">
-        <v>3928.2702834332799</v>
+        <v>3416.2177421309998</v>
       </c>
       <c r="E13">
-        <v>8269.9864942428194</v>
+        <v>12221.6368687757</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>5982.5545823574503</v>
+        <v>6890.7761984919198</v>
       </c>
       <c r="B14">
-        <v>4450.6043521168203</v>
+        <v>4146.0632011356302</v>
       </c>
       <c r="C14">
-        <v>7900.1293299218996</v>
+        <v>11054.992166926</v>
       </c>
       <c r="D14">
-        <v>4033.13908001653</v>
+        <v>3482.2210740588798</v>
       </c>
       <c r="E14">
-        <v>8601.2800907144101</v>
+        <v>12787.823053619901</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>6162.1640784062402</v>
+        <v>7089.2378469999703</v>
       </c>
       <c r="B15">
-        <v>4564.5133381487703</v>
+        <v>4229.2191148000002</v>
       </c>
       <c r="C15">
-        <v>8177.8086614026697</v>
+        <v>11488.426424779</v>
       </c>
       <c r="D15">
-        <v>4131.3598746260895</v>
+        <v>3543.61143940792</v>
       </c>
       <c r="E15">
-        <v>8918.6515668103602</v>
+        <v>13335.3122508694</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>6332.9371531999604</v>
+        <v>7278.1459844891097</v>
       </c>
       <c r="B16">
-        <v>4671.9564568580699</v>
+        <v>4307.2899635567301</v>
       </c>
       <c r="C16">
-        <v>8443.94416988591</v>
+        <v>11906.713714384699</v>
       </c>
       <c r="D16">
-        <v>4223.7730315589297</v>
+        <v>3600.9989336291801</v>
       </c>
       <c r="E16">
-        <v>9223.5935246100398</v>
+        <v>13865.9583983917</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>6495.84075180748</v>
+        <v>7458.5368605390004</v>
       </c>
       <c r="B17">
-        <v>4773.6855428201998</v>
+        <v>4380.8872426302196</v>
       </c>
       <c r="C17">
-        <v>8699.7194598306705</v>
+        <v>12311.3164711666</v>
       </c>
       <c r="D17">
-        <v>4311.0662923411301</v>
+        <v>3654.8796208451699</v>
       </c>
       <c r="E17">
-        <v>9517.3533376414198</v>
+        <v>14381.3242214273</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>6651.6845770098398</v>
+        <v>7631.2791151916099</v>
       </c>
       <c r="B18">
-        <v>4870.3254865839599</v>
+        <v>4450.5169860476799</v>
       </c>
       <c r="C18">
-        <v>8946.1330666469203</v>
+        <v>12703.4763780907</v>
       </c>
       <c r="D18">
-        <v>4393.8099351928304</v>
+        <v>3705.6623518072101</v>
       </c>
       <c r="E18">
-        <v>9800.9857974095394</v>
+        <v>14882.741863950099</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>6801.1540982311899</v>
+        <v>7797.1088311145604</v>
       </c>
       <c r="B19">
-        <v>4962.4016047894702</v>
+        <v>4516.6028536846097</v>
       </c>
       <c r="C19">
-        <v>9184.0362530941202</v>
+        <v>13084.2583663121</v>
       </c>
       <c r="D19">
-        <v>4472.4823103265298</v>
+        <v>3753.6881231491702</v>
       </c>
       <c r="E19">
-        <v>10075.392099569601</v>
+        <v>15371.358141222399</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>6944.8352335365598</v>
+        <v>7956.6557688509101</v>
       </c>
       <c r="B20">
-        <v>5050.3599633571102</v>
+        <v>4579.5032040918604</v>
       </c>
       <c r="C20">
-        <v>9414.16146756546</v>
+        <v>13454.583941081</v>
       </c>
       <c r="D20">
-        <v>4547.4887589964601</v>
+        <v>3799.2443391143102</v>
       </c>
       <c r="E20">
-        <v>10341.3492615342</v>
+        <v>15848.168939306899</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>7083.2331225985599</v>
+        <v>8110.4633394623897</v>
       </c>
       <c r="B21">
-        <v>5134.58273366919</v>
+        <v>4639.5239450135496</v>
       </c>
       <c r="C21">
-        <v>9637.1441313301293</v>
+        <v>13815.256838388699</v>
       </c>
       <c r="D21">
-        <v>4619.1758790530102</v>
+        <v>3842.57550774011</v>
       </c>
       <c r="E21">
-        <v>10599.532690188</v>
+        <v>16314.045790005101</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>7216.78662308611</v>
+        <v>8259.0040406778207</v>
       </c>
       <c r="B22">
-        <v>5215.3999768454596</v>
+        <v>4696.9283588928802</v>
       </c>
       <c r="C22">
-        <v>9853.5395670661201</v>
+        <v>14166.9830657781</v>
       </c>
       <c r="D22">
-        <v>4687.8424507893596</v>
+        <v>3883.8913914581299</v>
       </c>
       <c r="E22">
-        <v>10850.5337507982</v>
+        <v>16769.7566972282</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>7345.8796572430101</v>
+        <v>8402.6915489842304</v>
       </c>
       <c r="B23">
-        <v>5293.0988131020404</v>
+        <v>4751.9447216820599</v>
       </c>
       <c r="C23">
-        <v>10063.8363272849</v>
+        <v>14510.386760739</v>
       </c>
       <c r="D23">
-        <v>4753.7479225265897</v>
+        <v>3923.3733068565698</v>
       </c>
       <c r="E23">
-        <v>11094.8736250821</v>
+        <v>17215.982668585701</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>7470.8502018524896</v>
+        <v>8541.8903077712494</v>
       </c>
       <c r="B24">
-        <v>5367.9306459199097</v>
+        <v>4804.7722856585997</v>
       </c>
       <c r="C24">
-        <v>10268.4668138171</v>
+        <v>14846.0228866571</v>
       </c>
       <c r="D24">
-        <v>4817.1190842238202</v>
+        <v>3961.17905657335</v>
       </c>
       <c r="E24">
-        <v>11333.014372035401</v>
+        <v>17653.330989774699</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>7591.9974899221997</v>
+        <v>8676.9232139456799</v>
       </c>
       <c r="B25">
-        <v>5440.1169182085696</v>
+        <v>4855.5860315436103</v>
       </c>
       <c r="C25">
-        <v>10467.815830440901</v>
+        <v>15174.387504656101</v>
       </c>
       <c r="D25">
-        <v>4878.1553759814497</v>
+        <v>3997.4468352601598</v>
       </c>
       <c r="E25">
-        <v>11565.3678509047</v>
+        <v>18082.345995045602</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>7709.5878378581501</v>
+        <v>8808.0778419242106</v>
       </c>
       <c r="B26">
-        <v>5509.8537460220596</v>
+        <v>4904.5404825002897</v>
       </c>
       <c r="C26">
-        <v>10662.227538594499</v>
+        <v>15495.9261641665</v>
       </c>
       <c r="D26">
-        <v>4937.0331544946303</v>
+        <v>4032.2983557419798</v>
       </c>
       <c r="E26">
-        <v>11792.302989702301</v>
+        <v>18503.517889088798</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>7823.8594037605399</v>
+        <v>8935.6115294361207</v>
       </c>
       <c r="B27">
-        <v>5577.3156837740198</v>
+        <v>4951.7727943827404</v>
       </c>
       <c r="C27">
-        <v>10852.0111650578</v>
+        <v>15811.0408169605</v>
       </c>
       <c r="D27">
-        <v>4993.9091544861203</v>
+        <v>4065.8413752032302</v>
       </c>
       <c r="E27">
-        <v>12014.151758709</v>
+        <v>18917.2900355196</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>7935.0261055999199</v>
+        <v>9059.7555681306803</v>
       </c>
       <c r="B28">
-        <v>5642.6588100967001</v>
+        <v>4997.4052814446904</v>
       </c>
       <c r="C28">
-        <v>11037.4457240097</v>
+        <v>16120.095560329601</v>
       </c>
       <c r="D28">
-        <v>5048.9233213903799</v>
+        <v>4098.1717546030204</v>
       </c>
       <c r="E28">
-        <v>12231.2141197194</v>
+        <v>19324.065026318302</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>8043.2808725752902</v>
+        <v>9180.7186831959407</v>
       </c>
       <c r="B29">
-        <v>5706.0232769636996</v>
+        <v>5041.54749722625</v>
       </c>
       <c r="C29">
-        <v>11218.7839531791</v>
+        <v>16423.421442983901</v>
       </c>
       <c r="D29">
-        <v>5102.2011480056699</v>
+        <v>4129.3751512256204</v>
       </c>
       <c r="E29">
-        <v>12443.762157404701</v>
+        <v>19724.2097730356</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>8148.79836241049</v>
+        <v>9298.6899431873408</v>
       </c>
       <c r="B30">
-        <v>5767.5354308371698</v>
+        <v>5084.2979616736902</v>
       </c>
       <c r="C30">
-        <v>11396.255617770399</v>
+        <v>16721.320514100102</v>
       </c>
       <c r="D30">
-        <v>5153.85561617861</v>
+        <v>4159.5284201655204</v>
       </c>
       <c r="E30">
-        <v>12652.0435518179</v>
+        <v>20118.059806210302</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
-        <v>8251.7372473329306</v>
+        <v>9413.8412094102805</v>
       </c>
       <c r="B31">
-        <v>5827.3095896475998</v>
+        <v>5125.7456044783903</v>
       </c>
       <c r="C31">
-        <v>11570.070301617799</v>
+        <v>17014.0692562767</v>
       </c>
       <c r="D31">
-        <v>5203.9888212927699</v>
+        <v>4188.7007828706901</v>
       </c>
       <c r="E31">
-        <v>12856.284515815199</v>
+        <v>20505.922928794698</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>8352.2421490088</v>
+        <v>9526.3292103368294</v>
       </c>
       <c r="B32">
-        <v>5885.4495408121302</v>
+        <v>5165.9709789536801</v>
       </c>
       <c r="C32">
-        <v>11740.419779285199</v>
+        <v>17301.9215132235</v>
       </c>
       <c r="D32">
-        <v>5252.6933399901</v>
+        <v>4216.9548077522004</v>
       </c>
       <c r="E32">
-        <v>13056.692294627001</v>
+        <v>20888.082338629101</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>8450.4452857080905</v>
+        <v>9636.2973084714504</v>
       </c>
       <c r="B33">
-        <v>5942.0498114801503</v>
+        <v>5205.0472889906196</v>
       </c>
       <c r="C33">
-        <v>11907.4800432801</v>
+        <v>17585.1110001979</v>
       </c>
       <c r="D33">
-        <v>5300.0533885039904</v>
+        <v>4244.3472380329003</v>
       </c>
       <c r="E33">
-        <v>13253.457304625999</v>
+        <v>21264.7993115227</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>8546.4678819814799</v>
+        <v>9743.8770132683294</v>
       </c>
       <c r="B34">
-        <v>5997.1967515265997</v>
+        <v>5243.0412626908001</v>
       </c>
       <c r="C34">
-        <v>12071.4130455503</v>
+        <v>17863.853467631601</v>
       </c>
       <c r="D34">
-        <v>5346.1458090618999</v>
+        <v>4270.9296945543501</v>
       </c>
       <c r="E34">
-        <v>13446.7549728332</v>
+        <v>21636.315518373602</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>8640.4213811151803</v>
+        <v>9849.1892830474899</v>
       </c>
       <c r="B35">
-        <v>6050.96946161914</v>
+        <v>5280.0138994208201</v>
       </c>
       <c r="C35">
-        <v>12232.3682008252</v>
+        <v>18138.3485747591</v>
       </c>
       <c r="D35">
-        <v>5391.0409142052204</v>
+        <v>4296.7492755619596</v>
       </c>
       <c r="E35">
-        <v>13636.747326688201</v>
+        <v>22002.8550356667</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>8732.4084928386601</v>
+        <v>9952.3456505654194</v>
       </c>
       <c r="B36">
-        <v>6103.4405923356198</v>
+        <v>5316.0211117335502</v>
       </c>
       <c r="C36">
-        <v>12390.483690299799</v>
+        <v>18408.781519374199</v>
       </c>
       <c r="D36">
-        <v>5434.8032129836001</v>
+        <v>4321.8490710898104</v>
       </c>
       <c r="E36">
-        <v>13823.5843742178</v>
+        <v>22364.626097623499</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
-        <v>8822.5241026539807</v>
+        <v>10053.449200392801</v>
       </c>
       <c r="B37">
-        <v>6154.6770353490701</v>
+        <v>5351.1142794714497</v>
       </c>
       <c r="C37">
-        <v>12545.887597032301</v>
+        <v>18675.324461416101</v>
       </c>
       <c r="D37">
-        <v>5477.4920383852896</v>
+        <v>4346.2686061456398</v>
       </c>
       <c r="E37">
-        <v>14007.405307343201</v>
+        <v>22721.822629535101</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
-        <v>8910.8560643315395</v>
+        <v>10152.595421113099</v>
       </c>
       <c r="B38">
-        <v>6204.74052379357</v>
+        <v>5385.3407301223297</v>
       </c>
       <c r="C38">
-        <v>12698.698898774701</v>
+        <v>18938.137771385798</v>
       </c>
       <c r="D38">
-        <v>5519.1620917519904</v>
+        <v>4370.0442242139998</v>
       </c>
       <c r="E38">
-        <v>14188.339555196901</v>
+        <v>23074.625594841</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
-        <v>8997.4858932805892</v>
+        <v>10249.8729512667</v>
       </c>
       <c r="B39">
-        <v>6253.6881558300502</v>
+        <v>5418.7441569316297</v>
       </c>
       <c r="C39">
-        <v>12849.0283394462</v>
+        <v>19197.371129231698</v>
       </c>
       <c r="D39">
-        <v>5559.8639170655497</v>
+        <v>4393.2094204774103</v>
       </c>
       <c r="E39">
-        <v>14366.5077096319</v>
+        <v>23423.204182936301</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
-        <v>9082.4893754309705</v>
+        <v>10345.364234689099</v>
       </c>
       <c r="B40">
-        <v>6301.57285296173</v>
+        <v>5451.3649842306904</v>
       </c>
       <c r="C40">
-        <v>12996.979196837799</v>
+        <v>19453.1644950228</v>
       </c>
       <c r="D40">
-        <v>5599.6443157126396</v>
+        <v>4415.7951324713304</v>
       </c>
       <c r="E40">
-        <v>14542.0223413357</v>
+        <v>23767.716860177101</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
-        <v>9165.9371037873207</v>
+        <v>10439.1460982505</v>
       </c>
       <c r="B41">
-        <v>6348.4437626650797</v>
+        <v>5483.2406878013999</v>
       </c>
       <c r="C41">
-        <v>13142.6479612073</v>
+        <v>19705.648969226499</v>
       </c>
       <c r="D41">
-        <v>5638.5467105036596</v>
+        <v>4437.8299945408698</v>
       </c>
       <c r="E41">
-        <v>14714.988721913</v>
+        <v>24108.3123029009</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
-        <v>9247.8949528110497</v>
+        <v>10531.290262865999</v>
       </c>
       <c r="B42">
-        <v>6394.3466133002403</v>
+        <v>5514.4060767762103</v>
       </c>
       <c r="C42">
-        <v>13286.1249370433</v>
+        <v>19954.947557557</v>
       </c>
       <c r="D42">
-        <v>5676.6114662448199</v>
+        <v>4459.3405613821496</v>
       </c>
       <c r="E42">
-        <v>14885.5054648157</v>
+        <v>24445.1302282865</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
-        <v>9328.4244991504002</v>
+        <v>10621.8637968943</v>
       </c>
       <c r="B43">
-        <v>6439.3240279622196</v>
+        <v>5544.89354250006</v>
       </c>
       <c r="C43">
-        <v>13427.4947783318</v>
+        <v>20201.175853016</v>
       </c>
       <c r="D43">
-        <v>5713.8761729630096</v>
+        <v>4480.35150507243</v>
       </c>
       <c r="E43">
-        <v>15053.6650959702</v>
+        <v>24778.302136427999</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
-        <v>9407.5833958991207</v>
+        <v>10710.9295196188</v>
       </c>
       <c r="B44">
-        <v>6483.4158028708198</v>
+        <v>5574.7332789064203</v>
       </c>
       <c r="C44">
-        <v>13566.836966059</v>
+        <v>20444.4426458243</v>
       </c>
       <c r="D44">
-        <v>5750.3758969044902</v>
+        <v>4500.8857892778497</v>
       </c>
       <c r="E44">
-        <v>15219.554563280701</v>
+        <v>25107.9519749723</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
-        <v>9485.4257064611993</v>
+        <v>10798.546361319</v>
       </c>
       <c r="B45">
-        <v>6526.6591550232297</v>
+        <v>5603.9534782431401</v>
       </c>
       <c r="C45">
-        <v>13704.226235362399</v>
+        <v>20684.8504703459</v>
       </c>
       <c r="D45">
-        <v>5786.1434036254204</v>
+        <v>4520.9648237417296</v>
       </c>
       <c r="E45">
-        <v>15383.255692803699</v>
+        <v>25434.1967359917</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
-        <v>9562.0022031864992</v>
+        <v>10884.769685470699</v>
       </c>
       <c r="B46">
-        <v>6569.08894311329</v>
+        <v>5632.5805053931999</v>
       </c>
       <c r="C46">
-        <v>13839.732958649</v>
+        <v>20922.4960967794</v>
       </c>
       <c r="D46">
-        <v>5821.2093568301598</v>
+        <v>4540.6086016750896</v>
       </c>
       <c r="E46">
-        <v>15544.8455982463</v>
+        <v>25757.146993366201</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
-        <v>9637.3606351825492</v>
+        <v>10969.6515777965</v>
       </c>
       <c r="B47">
-        <v>6610.7378651229601</v>
+        <v>5660.6390535466599</v>
       </c>
       <c r="C47">
-        <v>13973.423490081201</v>
+        <v>21157.470974281601</v>
       </c>
       <c r="D47">
-        <v>5855.6024960651503</v>
+        <v>4559.8358222727302</v>
       </c>
       <c r="E47">
-        <v>15704.3970494806</v>
+        <v>26076.907387778301</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>9711.5459690755906</v>
+        <v>11053.2411062145</v>
       </c>
       <c r="B48">
-        <v>6651.6366354950896</v>
+        <v>5688.1522835742499</v>
       </c>
       <c r="C48">
-        <v>14105.360476072899</v>
+        <v>21389.861631260599</v>
       </c>
       <c r="D48">
-        <v>5889.3497959202396</v>
+        <v>4578.6640002479999</v>
       </c>
       <c r="E48">
-        <v>15861.9788049656</v>
+        <v>26393.577065443202</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
-        <v>9784.6006059616702</v>
+        <v>11135.584555162801</v>
       </c>
       <c r="B49">
-        <v>6691.8141443798904</v>
+        <v>5715.1419491137203</v>
       </c>
       <c r="C49">
-        <v>14235.603135789301</v>
+        <v>21619.750037788701</v>
       </c>
       <c r="D49">
-        <v>5922.4766090078501</v>
+        <v>4597.1095640039302</v>
       </c>
       <c r="E49">
-        <v>16017.6559122953</v>
+        <v>26707.250075866301</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
-        <v>9856.5645773425404</v>
+        <v>11216.725637298699</v>
       </c>
       <c r="B50">
-        <v>6731.2976010990296</v>
+        <v>5741.6285090957399</v>
       </c>
       <c r="C50">
-        <v>14364.207515104699</v>
+        <v>21847.213934425701</v>
       </c>
       <c r="D50">
-        <v>5955.0067946713698</v>
+        <v>4615.1879438277601</v>
       </c>
       <c r="E50">
-        <v>16171.4899805201</v>
+        <v>27018.015733218399</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
-        <v>9927.4757224632503</v>
+        <v>11296.705685168699</v>
       </c>
       <c r="B51">
-        <v>6770.1126636764502</v>
+        <v>5767.6312291971999</v>
       </c>
       <c r="C51">
-        <v>14491.226717015499</v>
+        <v>22072.3271311797</v>
       </c>
       <c r="D51">
-        <v>5986.9628351045403</v>
+        <v>4632.9136513023795</v>
       </c>
       <c r="E51">
-        <v>16323.539427408101</v>
+        <v>27325.9589453238</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
-        <v>9997.3698491482992</v>
+        <v>11375.563825101201</v>
       </c>
       <c r="B52">
-        <v>6808.2835560367303</v>
+        <v>5793.1682735076502</v>
       </c>
       <c r="C52">
-        <v>14616.7111111092</v>
+        <v>22295.159779852998</v>
       </c>
       <c r="D52">
-        <v>6018.3659403366701</v>
+        <v>4650.3003509646096</v>
       </c>
       <c r="E52">
-        <v>16473.8597044001</v>
+        <v>27631.1605137447</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
-        <v>10066.280879960599</v>
+        <v>11453.337135281599</v>
       </c>
       <c r="B53">
-        <v>6845.8331742602204</v>
+        <v>5818.2567875232698</v>
       </c>
       <c r="C53">
-        <v>14740.708524363799</v>
+        <v>22515.778622611699</v>
       </c>
       <c r="D53">
-        <v>6049.2361433450797</v>
+        <v>4667.3609251020198</v>
       </c>
       <c r="E53">
-        <v>16622.5035016648</v>
+        <v>27933.697408014399</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
-        <v>10134.240985275799</v>
+        <v>11530.0607897222</v>
       </c>
       <c r="B54">
-        <v>6882.7831831045396</v>
+        <v>5842.9129734375301</v>
       </c>
       <c r="C54">
-        <v>14863.2644152633</v>
+        <v>22734.247219267101</v>
       </c>
       <c r="D54">
-        <v>6079.59238639261</v>
+        <v>4684.1075324625099</v>
       </c>
       <c r="E54">
-        <v>16769.520935357101</v>
+        <v>28233.643016692698</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
-        <v>10201.280704663901</v>
+        <v>11605.768189623401</v>
       </c>
       <c r="B55">
-        <v>6919.1541038482201</v>
+        <v>5867.1521585730097</v>
       </c>
       <c r="C55">
-        <v>14984.422032971401</v>
+        <v>22950.626155456001</v>
       </c>
       <c r="D55">
-        <v>6109.4525995475296</v>
+        <v>4700.5516615508805</v>
       </c>
       <c r="E55">
-        <v>16914.959718928501</v>
+        <v>28531.067377600601</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
-        <v>10267.429057801901</v>
+        <v>11680.4910834413</v>
       </c>
       <c r="B56">
-        <v>6954.9653943808098</v>
+        <v>5890.9888576929097</v>
       </c>
       <c r="C56">
-        <v>15104.2225630958</v>
+        <v>23164.973233642399</v>
       </c>
       <c r="D56">
-        <v>6138.8337722231499</v>
+        <v>4716.7041791008196</v>
       </c>
       <c r="E56">
-        <v>17058.865320112502</v>
+        <v>28826.0373893094</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
-        <v>10332.713645989401</v>
+        <v>11754.2596768165</v>
       </c>
       <c r="B57">
-        <v>6990.2355223501499</v>
+        <v>5914.4368298393401</v>
       </c>
       <c r="C57">
-        <v>15222.705261392601</v>
+        <v>23377.343648644499</v>
       </c>
       <c r="D57">
-        <v>6167.7520184717596</v>
+        <v>4732.57537423756</v>
       </c>
       <c r="E57">
-        <v>17201.2811050206</v>
+        <v>29118.6170057196</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
-        <v>10397.160745217499</v>
+        <v>11827.1027333853</v>
       </c>
       <c r="B58">
-        <v>7024.9820320803501</v>
+        <v>5937.5091302667197</v>
       </c>
       <c r="C58">
-        <v>15339.9075766033</v>
+        <v>23587.790149189401</v>
       </c>
       <c r="D58">
-        <v>6196.2226366780496</v>
+        <v>4748.17499878325</v>
       </c>
       <c r="E58">
-        <v>17342.248470614501</v>
+        <v>29408.867415357301</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
-        <v>10460.795391625399</v>
+        <v>11899.047667373001</v>
       </c>
       <c r="B59">
-        <v>7059.2216058894601</v>
+        <v>5960.2181579712396</v>
       </c>
       <c r="C59">
-        <v>15455.865263482699</v>
+        <v>23796.363186832001</v>
       </c>
       <c r="D59">
-        <v>6224.2601642212003</v>
+        <v>4763.51230410277</v>
       </c>
       <c r="E59">
-        <v>17481.806966677799</v>
+        <v>29696.847206833001</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
-        <v>10523.641460088</v>
+        <v>11970.1206287679</v>
       </c>
       <c r="B60">
-        <v>7092.9701203626</v>
+        <v>5982.57569925799</v>
       </c>
       <c r="C60">
-        <v>15570.6124869512</v>
+        <v>24003.111053424502</v>
       </c>
       <c r="D60">
-        <v>6251.8784276076103</v>
+        <v>4778.5960748405196</v>
       </c>
       <c r="E60">
-        <v>17619.994408283801</v>
+        <v>29982.6125217472</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
-        <v>10585.7217365913</v>
+        <v>12040.346581785299</v>
       </c>
       <c r="B61">
-        <v>7126.2426980730697</v>
+        <v>6004.5929677369504</v>
       </c>
       <c r="C61">
-        <v>15684.181918209</v>
+        <v>24208.0800081938</v>
       </c>
       <c r="D61">
-        <v>6279.0905885193597</v>
+        <v>4793.4346598581697</v>
       </c>
       <c r="E61">
-        <v>17756.846979647999</v>
+        <v>30266.217196192101</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
-        <v>10647.0579849809</v>
+        <v>12109.7493772503</v>
       </c>
       <c r="B62">
-        <v>7159.0537551880998</v>
+        <v>6026.2806410942203</v>
       </c>
       <c r="C62">
-        <v>15796.604823551999</v>
+        <v>24411.314395370799</v>
       </c>
       <c r="D62">
-        <v>6305.90918617229</v>
+        <v>4808.0360006474803</v>
       </c>
       <c r="E62">
-        <v>17892.3993301544</v>
+        <v>30547.712891870498</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
-        <v>10707.671008605301</v>
+        <v>12178.3518194637</v>
       </c>
       <c r="B63">
-        <v>7191.4170453483302</v>
+        <v>6047.6488949464601</v>
       </c>
       <c r="C63">
-        <v>15907.911146554199</v>
+        <v>24612.8567532163</v>
       </c>
       <c r="D63">
-        <v>6332.3461763346904</v>
+        <v>4822.4076574619603</v>
       </c>
       <c r="E63">
-        <v>18026.684663263699</v>
+        <v>30827.149217753798</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
-        <v>10767.580707319101</v>
+        <v>12246.175728050401</v>
       </c>
       <c r="B64">
-        <v>7223.3457001669603</v>
+        <v>6068.7074340526196</v>
       </c>
       <c r="C64">
-        <v>16018.129584210001</v>
+        <v>24812.747915199001</v>
       </c>
       <c r="D64">
-        <v>6358.4129673186299</v>
+        <v>4836.55683338364</v>
       </c>
       <c r="E64">
-        <v>18159.7348189369</v>
+        <v>31104.5738430987</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
-        <v>10826.8061302637</v>
+        <v>12313.241995241</v>
       </c>
       <c r="B65">
-        <v>7254.8522666580802</v>
+        <v>6089.4655211274303</v>
       </c>
       <c r="C65">
-        <v>16127.2876575669</v>
+        <v>25011.027104006302</v>
       </c>
       <c r="D65">
-        <v>6384.1204532225202</v>
+        <v>4850.4903965180802</v>
       </c>
       <c r="E65">
-        <v>18291.580350139699</v>
+        <v>31380.032602564501</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
-        <v>10885.3655247969</v>
+        <v>12379.5706389886</v>
       </c>
       <c r="B66">
-        <v>7285.9487418705603</v>
+        <v>6109.9320034748098</v>
       </c>
       <c r="C66">
-        <v>16235.411777327499</v>
+        <v>25207.732018997001</v>
       </c>
       <c r="D66">
-        <v>6409.4790446739498</v>
+        <v>4864.21490048943</v>
       </c>
       <c r="E66">
-        <v>18422.250593939101</v>
+        <v>31653.569594095701</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
-        <v>10943.276381907999</v>
+        <v>12445.180852282299</v>
       </c>
       <c r="B67">
-        <v>7316.64660497563</v>
+        <v>6130.1153376370003</v>
       </c>
       <c r="C67">
-        <v>16342.5273048498</v>
+        <v>25402.898917647399</v>
       </c>
       <c r="D67">
-        <v>6434.4986972959396</v>
+        <v>4877.7366033900398</v>
       </c>
       <c r="E67">
-        <v>18551.773737650801</v>
+        <v>31925.227270171399</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
-        <v>11000.555478419499</v>
+        <v>12510.0910489831</v>
       </c>
       <c r="B68">
-        <v>7346.9568470304703</v>
+        <v>6150.0236122345796</v>
       </c>
       <c r="C68">
-        <v>16448.658608932201</v>
+        <v>25596.562691487401</v>
       </c>
       <c r="D68">
-        <v>6459.1889380966804</v>
+        <v>4891.0614853219904</v>
       </c>
       <c r="E68">
-        <v>18680.176880450701</v>
+        <v>32195.046522962701</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
-        <v>11057.2189162461</v>
+        <v>12574.3189064736</v>
       </c>
       <c r="B69">
-        <v>7376.8899986178403</v>
+        <v>6169.6645691547401</v>
       </c>
       <c r="C69">
-        <v>16553.829118733101</v>
+        <v>25788.756936973401</v>
       </c>
       <c r="D69">
-        <v>6483.55888996248</v>
+        <v>4904.1952646547197</v>
       </c>
       <c r="E69">
-        <v>18807.486090823</v>
+        <v>32463.066763889499</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
-        <v>11113.282158956899</v>
+        <v>12637.8814053884</v>
       </c>
       <c r="B70">
-        <v>7406.4561555422397</v>
+        <v>6189.0456232297201</v>
       </c>
       <c r="C70">
-        <v>16658.061373140499</v>
+        <v>25979.5140217074</v>
       </c>
       <c r="D70">
-        <v>6507.6172944159798</v>
+        <v>4917.1434131098204</v>
       </c>
       <c r="E70">
-        <v>18933.726460185098</v>
+        <v>32729.325998021999</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
-        <v>11168.760065861101</v>
+        <v>12700.7948666623</v>
       </c>
       <c r="B71">
-        <v>7435.6650027447604</v>
+        <v>6208.1738805328496</v>
       </c>
       <c r="C71">
-        <v>16761.377066876401</v>
+        <v>26168.865146367702</v>
       </c>
       <c r="D71">
-        <v>6531.37253278547</v>
+        <v>4929.9111697732396</v>
       </c>
       <c r="E71">
-        <v>19058.922152992302</v>
+        <v>32993.860893728299</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
-        <v>11223.6669238182</v>
+        <v>12763.0749861124</v>
       </c>
       <c r="B72">
-        <v>7464.5258365837999</v>
+        <v>6227.0561554075402</v>
       </c>
       <c r="C72">
-        <v>16863.797093596801</v>
+        <v>26356.840402686801</v>
       </c>
       <c r="D72">
-        <v>6554.8326459171003</v>
+        <v>4942.50355412513</v>
       </c>
       <c r="E72">
-        <v>19183.096453602098</v>
+        <v>33256.706847937203</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
-        <v>11278.016476954501</v>
+        <v>12824.736866752301</v>
       </c>
       <c r="B73">
-        <v>7493.0475856141802</v>
+        <v>6245.6989863333301</v>
       </c>
       <c r="C73">
-        <v>16965.3415862199</v>
+        <v>26543.468827780001</v>
       </c>
       <c r="D73">
-        <v>6578.0053525490803</v>
+        <v>4954.9253781689004</v>
       </c>
       <c r="E73">
-        <v>19306.2718101475</v>
+        <v>33517.8980473466</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
-        <v>11331.8219544491</v>
+        <v>12885.795049013999</v>
       </c>
       <c r="B74">
-        <v>7521.2388299855502</v>
+        <v>6264.1086507233504</v>
       </c>
       <c r="C74">
-        <v>17066.029954699199</v>
+        <v>26728.778455102802</v>
       </c>
       <c r="D74">
-        <v>6600.8980664560304</v>
+        <v>4967.1812577334804</v>
       </c>
       <c r="E74">
-        <v>19428.469875651801</v>
+        <v>33777.467525885797</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
-        <v>11385.0960965412</v>
+        <v>12946.2635390411</v>
       </c>
       <c r="B75">
-        <v>7549.1078195685805</v>
+        <v>6282.2911787384801</v>
       </c>
       <c r="C75">
-        <v>17165.880921432501</v>
+        <v>26912.796362286001</v>
       </c>
       <c r="D75">
-        <v>6623.5179124609604</v>
+        <v>4979.2756230150999</v>
       </c>
       <c r="E75">
-        <v>19549.711546590301</v>
+        <v>34035.447218703899</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
-        <v>11437.851178893001</v>
+        <v>13006.155835199501</v>
       </c>
       <c r="B76">
-        <v>7576.6624909090697</v>
+        <v>6300.2523661960204</v>
       </c>
       <c r="C76">
-        <v>17264.912554487899</v>
+        <v>27095.5487160837</v>
       </c>
       <c r="D76">
-        <v>6645.8717414042203</v>
+        <v>4991.2127284197304</v>
       </c>
       <c r="E76">
-        <v>19670.016999091298</v>
+        <v>34291.868012942497</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
-        <v>11490.099035434199</v>
+        <v>13065.4849529407</v>
       </c>
       <c r="B77">
-        <v>7603.9104830995302</v>
+        <v>6317.99778664323</v>
       </c>
       <c r="C77">
-        <v>17363.1422988058</v>
+        <v>27277.060814639601</v>
       </c>
       <c r="D77">
-        <v>6667.9661441498301</v>
+        <v>5002.9966617609098</v>
       </c>
       <c r="E77">
-        <v>19789.405722950502</v>
+        <v>34546.759795521801</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
-        <v>11541.851079799701</v>
+        <v>13124.2634481395</v>
       </c>
       <c r="B78">
-        <v>7630.8591526508299</v>
+        <v>6335.53280265989</v>
       </c>
       <c r="C78">
-        <v>17460.587005526198</v>
+        <v>27457.3571272679</v>
       </c>
       <c r="D78">
-        <v>6689.8074647030598</v>
+        <v>5014.6313528629098</v>
       </c>
       <c r="E78">
-        <v>19907.896553615799</v>
+        <v>34800.151498151601</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
-        <v>11593.118325465</v>
+        <v>13182.503439018399</v>
       </c>
       <c r="B79">
-        <v>7657.5155874390503</v>
+        <v>6352.8625764485296</v>
       </c>
       <c r="C79">
-        <v>17557.262959576001</v>
+        <v>27636.461331922699</v>
       </c>
       <c r="D79">
-        <v>6711.4018125061702</v>
+        <v>5026.1205816151096</v>
       </c>
       <c r="E79">
-        <v>20025.5077022898</v>
+        <v>35052.071139765001</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
-        <v>11643.9114046742</v>
+        <v>13240.216626762</v>
       </c>
       <c r="B80">
-        <v>7683.8866197957996</v>
+        <v>6369.9920797655705</v>
       </c>
       <c r="C80">
-        <v>17653.1859056414</v>
+        <v>27814.396350520499</v>
       </c>
       <c r="D80">
-        <v>6732.7550739737899</v>
+        <v>5037.4679855188597</v>
       </c>
       <c r="E80">
-        <v>20142.256784282901</v>
+        <v>35302.545866551103</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
-        <v>11694.2405862462</v>
+        <v>13297.414314912699</v>
       </c>
       <c r="B81">
-        <v>7709.97883880477</v>
+        <v>6386.9261032421</v>
       </c>
       <c r="C81">
-        <v>17748.371072637201</v>
+        <v>27991.184382260901</v>
       </c>
       <c r="D81">
-        <v>6753.8729233235699</v>
+        <v>5048.6770667648998</v>
       </c>
       <c r="E81">
-        <v>20258.160845738901</v>
+        <v>35551.601989750801</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
-        <v>11744.1157923394</v>
+        <v>13354.1074276375</v>
       </c>
       <c r="B82">
-        <v>7735.7986018620104</v>
+        <v>6403.6692651390504</v>
       </c>
       <c r="C82">
-        <v>17842.833196779698</v>
+        <v>28166.846935085599</v>
       </c>
       <c r="D82">
-        <v>6774.76083275367</v>
+        <v>5059.7511988758097</v>
       </c>
       <c r="E82">
-        <v>20373.2363888461</v>
+        <v>35799.265021368599</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
-        <v>11793.5466142477</v>
+        <v>13410.3065269408</v>
       </c>
       <c r="B83">
-        <v>7761.3520455521002</v>
+        <v>6420.2260195772797</v>
       </c>
       <c r="C83">
-        <v>17936.586543356399</v>
+        <v>28341.404855398599</v>
       </c>
       <c r="D83">
-        <v>6795.4240820136401</v>
+        <v>5070.6936329454202</v>
       </c>
       <c r="E83">
-        <v>20487.4993956363</v>
+        <v>36045.5597079371</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
-        <v>11842.542327294501</v>
+        <v>13466.0218288991</v>
       </c>
       <c r="B84">
-        <v>7786.64509588901</v>
+        <v>6436.6006642803704</v>
       </c>
       <c r="C84">
-        <v>18029.644927284298</v>
+        <v>28514.8783561657</v>
       </c>
       <c r="D84">
-        <v>6815.86776741208</v>
+        <v>5081.50750350405</v>
       </c>
       <c r="E84">
-        <v>20600.965350468701</v>
+        <v>36290.510062465502</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
-        <v>11891.111904887</v>
+        <v>13521.2632189821</v>
       </c>
       <c r="B85">
-        <v>7811.6834779652499</v>
+        <v>6452.7973478641297</v>
       </c>
       <c r="C85">
-        <v>18122.0217325339</v>
+        <v>28687.287043497799</v>
       </c>
       <c r="D85">
-        <v>6836.0968103001796</v>
+        <v>5092.1958340361798</v>
       </c>
       <c r="E85">
-        <v>20713.649261283299</v>
+        <v>36534.139394687198</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
-        <v>11939.264031786401</v>
+        <v>13576.0402665233</v>
       </c>
       <c r="B86">
-        <v>7836.4727250507303</v>
+        <v>6468.8200767046301</v>
       </c>
       <c r="C86">
-        <v>18213.729930497899</v>
+        <v>28858.6499418192</v>
       </c>
       <c r="D86">
-        <v>6856.1159650678101</v>
+        <v>5102.7615421751998</v>
       </c>
       <c r="E86">
-        <v>20825.565679708201</v>
+        <v>36776.470339718602</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
-        <v>11987.007116647799</v>
+        <v>13630.362238395601</v>
       </c>
       <c r="B87">
-        <v>7861.0181871782397</v>
+        <v>6484.6727214135499</v>
       </c>
       <c r="C87">
-        <v>18304.782097371099</v>
+        <v>29028.985517710498</v>
       </c>
       <c r="D87">
-        <v>6875.9298266852202</v>
+        <v>5113.2074445974404</v>
       </c>
       <c r="E87">
-        <v>20936.728720093401</v>
+        <v>37017.524885229599</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
-        <v>12034.349303876201</v>
+        <v>13684.2381119445</v>
       </c>
       <c r="B88">
-        <v>7885.3250392502196</v>
+        <v>6500.3590229476604</v>
       </c>
       <c r="C88">
-        <v>18395.190430606501</v>
+        <v>29198.311702508701</v>
       </c>
       <c r="D88">
-        <v>6895.54283782121</v>
+        <v>5123.5362616362299</v>
       </c>
       <c r="E88">
-        <v>21047.1520775387</v>
+        <v>37257.324397216602</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
-        <v>12081.2984848453</v>
+        <v>13737.676587227401</v>
       </c>
       <c r="B89">
-        <v>7909.3982886989197</v>
+        <v>6515.8825983770002</v>
       </c>
       <c r="C89">
-        <v>18484.966764506102</v>
+        <v>29366.645913747099</v>
       </c>
       <c r="D89">
-        <v>6914.9592955662301</v>
+        <v>5133.7506216351103</v>
       </c>
       <c r="E89">
-        <v>21156.849044983999</v>
+        <v>37495.889644470502</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
-        <v>12127.862308518001</v>
+        <v>13790.686098603899</v>
       </c>
       <c r="B90">
-        <v>7933.2427827289403</v>
+        <v>6531.2469463345697</v>
       </c>
       <c r="C90">
-        <v>18574.1225850023</v>
+        <v>29534.005075502901</v>
       </c>
       <c r="D90">
-        <v>6934.1833577862799</v>
+        <v>5143.8530650575804</v>
       </c>
       <c r="E90">
-        <v>21265.832529416399</v>
+        <v>37733.240821814397</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
-        <v>12174.0481915088</v>
+        <v>13843.274825717301</v>
       </c>
       <c r="B91">
-        <v>7956.8632151694901</v>
+        <v>6546.4554521681202</v>
       </c>
       <c r="C91">
-        <v>18662.669043678699</v>
+        <v>29700.4056377204</v>
       </c>
       <c r="D91">
-        <v>6953.2190491319798</v>
+        <v>5153.8460483694998</v>
       </c>
       <c r="E91">
-        <v>21374.115067251001</v>
+        <v>37969.3975721881</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
-        <v>12219.863327621501</v>
+        <v>13895.450703906999</v>
       </c>
       <c r="B92">
-        <v>7980.2641329614698</v>
+        <v>6561.5113928139299</v>
       </c>
       <c r="C92">
-        <v>18750.6169710791</v>
+        <v>29865.863594574901</v>
       </c>
       <c r="D92">
-        <v>6972.0702667250398</v>
+        <v>5163.7319477093797</v>
       </c>
       <c r="E92">
-        <v>21481.708838936502</v>
+        <v>38204.379007650103</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
-        <v>12265.314696896799</v>
+        <v>13947.221434085999</v>
       </c>
       <c r="B93">
-        <v>8003.44994230266</v>
+        <v>6576.4179414099899</v>
       </c>
       <c r="C93">
-        <v>18837.976889347501</v>
+        <v>30030.394501931802</v>
       </c>
       <c r="D93">
-        <v>6990.74078554277</v>
+        <v>5173.5130623599298</v>
       </c>
       <c r="E93">
-        <v>21588.625682832699</v>
+        <v>38438.203729359397</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
-        <v>12310.4090741975</v>
+        <v>13998.594492117199</v>
       </c>
       <c r="B94">
-        <v>8026.4249144721498</v>
+        <v>6591.1781716653604</v>
       </c>
       <c r="C94">
-        <v>18924.759024238501</v>
+        <v>30194.013493954801</v>
       </c>
       <c r="D94">
-        <v>7009.2342635196201</v>
+        <v>5183.1916180339604</v>
       </c>
       <c r="E94">
-        <v>21694.877108401499</v>
+        <v>38670.889846596001</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
-        <v>12355.153037362599</v>
+        <v>14049.577137718499</v>
       </c>
       <c r="B95">
-        <v>8049.1931913545704</v>
+        <v>6605.7950620011297</v>
       </c>
       <c r="C95">
-        <v>19010.9733165383</v>
+        <v>30356.735298916101</v>
       </c>
       <c r="D95">
-        <v>7027.5542463837901</v>
+        <v>5192.7697699862401</v>
       </c>
       <c r="E95">
-        <v>21800.4743087555</v>
+        <v>38902.454994880201</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
-        <v>12399.5529749542</v>
+        <v>14100.176422925701</v>
       </c>
       <c r="B96">
-        <v>8071.75879068224</v>
+        <v>6620.2714994770604</v>
       </c>
       <c r="C96">
-        <v>19096.629432928999</v>
+        <v>30518.574254252399</v>
       </c>
       <c r="D96">
-        <v>7045.7041722450103</v>
+        <v>5202.24960596251</v>
       </c>
       <c r="E96">
-        <v>21905.428172600401</v>
+        <v>39132.916353240202</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
-        <v>12443.6150936214</v>
+        <v>14150.3992001388</v>
       </c>
       <c r="B97">
-        <v>8094.1256110122404</v>
+        <v>6634.6102835170996</v>
       </c>
       <c r="C97">
-        <v>19181.736776329199</v>
+        <v>30679.544320909899</v>
       </c>
       <c r="D97">
-        <v>7063.6873759487798</v>
+        <v>5211.63314899532</v>
       </c>
       <c r="E97">
-        <v>22009.749295605001</v>
+        <v>39362.290660672603</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
-        <v>12487.345425105899</v>
+        <v>14200.2521297769</v>
       </c>
       <c r="B98">
-        <v>8116.29743645502</v>
+        <v>6648.8141294462703</v>
       </c>
       <c r="C98">
-        <v>19266.304495742599</v>
+        <v>30839.6590970221</v>
       </c>
       <c r="D98">
-        <v>7081.5070932115204</v>
+        <v>5220.9223600567902</v>
       </c>
       <c r="E98">
-        <v>22113.447991235698</v>
+        <v>39590.594231850897</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
-        <v>12530.749832908399</v>
+        <v>14249.741687564099</v>
       </c>
       <c r="B99">
-        <v>8138.2779411687598</v>
+        <v>6662.8856718500301</v>
       </c>
       <c r="C99">
-        <v>19350.341495641202</v>
+        <v>30998.931830953999</v>
       </c>
       <c r="D99">
-        <v>7099.1664645494402</v>
+        <v>5230.1191405764002</v>
       </c>
       <c r="E99">
-        <v>22216.534301081501</v>
+        <v>39817.842972113896</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
-        <v>12573.8340186351</v>
+        <v>14298.8741714684</v>
       </c>
       <c r="B100">
-        <v>8160.0706936335901</v>
+        <v>6676.8274677668096</v>
       </c>
       <c r="C100">
-        <v>19433.856444910201</v>
+        <v>31157.3754337504</v>
       </c>
       <c r="D100">
-        <v>7116.6685390135699</v>
+        <v>5239.2253348323102</v>
       </c>
       <c r="E100">
-        <v>22319.018004701898</v>
+        <v>40044.052391778998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>